<commit_message>
1.Matrix rotation 2.Overlap values in matrix
</commit_message>
<xml_diff>
--- a/tracker/solution tracker.xlsx
+++ b/tracker/solution tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose_\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LeetCode\tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B9A176-55C0-4B5F-B3B0-E21202802B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E66E001-0260-4E41-80AF-27AE898101B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20664" yWindow="192" windowWidth="20472" windowHeight="16296" tabRatio="1000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="1000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="147">
   <si>
     <t>Each sheet of this spreadsheet contains a leetcode pattern. While these questions aren't an exhaustive list of all leetcode questions, if you are able to  go through these questions with relative ease, most leetode questions should come relatively easy for you.</t>
   </si>
@@ -480,12 +480,21 @@
   <si>
     <t>Good Array</t>
   </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combinar DS y usar prefix sum para checar cuando values se empalman, en vez de usar un hashmap. </t>
+  </si>
+  <si>
+    <t>Rotate and Swap Matrix are basic utils we need to dominate. For 2D and 1D arrays.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +561,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -573,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -603,28 +618,13 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -695,6 +695,23 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -709,17 +726,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B6A23272-7EC8-4C33-9B29-E95BE43DA10B}" name="Tabla1" displayName="Tabla1" ref="A1:K41" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B6A23272-7EC8-4C33-9B29-E95BE43DA10B}" name="Tabla1" displayName="Tabla1" ref="A1:K41" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:K41" xr:uid="{B6A23272-7EC8-4C33-9B29-E95BE43DA10B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B96261EB-ECE6-4B5C-A81E-64BBE2B947B6}" name="Date Solved"/>
-    <tableColumn id="2" xr3:uid="{3AB7BFFC-8B43-4D5B-9149-3B9D42598D82}" name="Problem No" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{62BC8655-30E5-4560-B5B4-135B3D28ACB8}" name="Problem Title" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{798A31DC-25D4-4B25-9104-FC0CBE680529}" name="Difficulty" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{3AB7BFFC-8B43-4D5B-9149-3B9D42598D82}" name="Problem No" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{62BC8655-30E5-4560-B5B4-135B3D28ACB8}" name="Problem Title" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{798A31DC-25D4-4B25-9104-FC0CBE680529}" name="Difficulty" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{AB3D7EDA-8044-40F1-895E-DAD4F4045B61}" name="Notes"/>
     <tableColumn id="6" xr3:uid="{B7F3AFD5-BCB5-401A-BB4A-3B214E7A8E34}" name="Solved First Time? (Y/N)"/>
-    <tableColumn id="7" xr3:uid="{7E4173D8-49CF-4E20-A013-5EE1BF32FCD3}" name="Next Solve Date" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{DCD5B3BC-021D-401C-934C-2497EB1A47C0}" name="Next Solved Date"/>
+    <tableColumn id="7" xr3:uid="{7E4173D8-49CF-4E20-A013-5EE1BF32FCD3}" name="Next Solve Date" dataDxfId="0">
+      <calculatedColumnFormula>DATE(YEAR(A2),MONTH(A2),DAY(A2) + IF(F2 = "Y", 14, 7))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{DCD5B3BC-021D-401C-934C-2497EB1A47C0}" name="Next Solved Date">
+      <calculatedColumnFormula>DATE(YEAR(G2),MONTH(G2),DAY(G2)+7)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="9" xr3:uid="{F4D2895B-29FB-4474-9AB1-EB1AFBE9684D}" name="Next Solve Date2"/>
     <tableColumn id="10" xr3:uid="{15DCE018-5FC4-4950-80C3-D059C3626CF1}" name="Next Solve Date3"/>
     <tableColumn id="11" xr3:uid="{FC231F34-94A2-4518-8B32-E4AC07DCB074}" name="IsProblemCompetent"/>
@@ -8365,7 +8386,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8373,9 +8394,9 @@
     <col min="1" max="2" width="11.296875" customWidth="1"/>
     <col min="3" max="3" width="42.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.59765625" customWidth="1"/>
-    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="5" max="5" width="76.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.8984375" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.796875" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.19921875" customWidth="1"/>
     <col min="9" max="10" width="13.3984375" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="18.09765625" customWidth="1"/>
@@ -8451,6 +8472,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
       <c r="B3" s="7">
         <v>1929</v>
       </c>
@@ -8460,9 +8482,17 @@
       <c r="D3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G41" si="0">DATE(YEAR(A3),MONTH(A3),DAY(A3) + IF(F3 = "Y", 14, 7))</f>
+        <v>7</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H41" si="1">DATE(YEAR(G3),MONTH(G3),DAY(G3)+7)</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="17"/>
       <c r="B4" s="7"/>
       <c r="C4" s="13" t="s">
         <v>109</v>
@@ -8470,9 +8500,17 @@
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
       <c r="B5" s="7"/>
       <c r="C5" s="13" t="s">
         <v>110</v>
@@ -8480,9 +8518,17 @@
       <c r="D5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
       <c r="B6" s="7"/>
       <c r="C6" s="13" t="s">
         <v>111</v>
@@ -8490,9 +8536,17 @@
       <c r="D6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
       <c r="B7" s="7"/>
       <c r="C7" s="13" t="s">
         <v>112</v>
@@ -8500,9 +8554,17 @@
       <c r="D7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
       <c r="B8" s="7"/>
       <c r="C8" s="13" t="s">
         <v>134</v>
@@ -8511,9 +8573,17 @@
         <v>22</v>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
       <c r="B9" s="7"/>
       <c r="C9" s="13" t="s">
         <v>133</v>
@@ -8521,9 +8591,17 @@
       <c r="D9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13" t="s">
         <v>113</v>
@@ -8531,9 +8609,17 @@
       <c r="D10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13" t="s">
         <v>132</v>
@@ -8541,9 +8627,17 @@
       <c r="D11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="8"/>
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13" t="s">
         <v>114</v>
@@ -8551,10 +8645,17 @@
       <c r="D12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="8"/>
+      <c r="G12" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
         <v>115</v>
@@ -8563,10 +8664,17 @@
         <v>22</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="G13" s="8"/>
+      <c r="G13" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
         <v>118</v>
@@ -8575,10 +8683,17 @@
         <v>22</v>
       </c>
       <c r="E14" s="13"/>
-      <c r="G14" s="14"/>
+      <c r="G14" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
         <v>119</v>
@@ -8588,10 +8703,17 @@
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
         <v>120</v>
@@ -8599,12 +8721,19 @@
       <c r="D16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
+      <c r="G16" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H16" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13" t="s">
         <v>121</v>
@@ -8614,10 +8743,18 @@
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="G17" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H17" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
         <v>122</v>
@@ -8627,10 +8764,19 @@
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+      <c r="G18" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H18" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>44603</v>
+      </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13" t="s">
         <v>123</v>
@@ -8638,12 +8784,28 @@
       <c r="D19" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="E19" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G19" s="8">
+        <f t="shared" si="0"/>
+        <v>44610</v>
+      </c>
+      <c r="H19" s="8">
+        <f t="shared" si="1"/>
+        <v>44617</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <v>44603</v>
+      </c>
       <c r="B20" s="13"/>
       <c r="C20" s="13" t="s">
         <v>124</v>
@@ -8651,12 +8813,26 @@
       <c r="D20" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
+      <c r="E20" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="0"/>
+        <v>44610</v>
+      </c>
+      <c r="H20" s="8">
+        <f t="shared" si="1"/>
+        <v>44617</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13" t="s">
         <v>131</v>
@@ -8666,10 +8842,17 @@
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+      <c r="G21" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H21" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13" t="s">
         <v>125</v>
@@ -8679,10 +8862,17 @@
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+      <c r="G22" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H22" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13" t="s">
         <v>126</v>
@@ -8692,10 +8882,17 @@
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="G23" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H23" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13" t="s">
         <v>77</v>
@@ -8705,10 +8902,17 @@
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="G24" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13" t="s">
         <v>127</v>
@@ -8718,10 +8922,17 @@
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="14"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+      <c r="G25" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H25" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13" t="s">
         <v>128</v>
@@ -8731,10 +8942,17 @@
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+      <c r="G26" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H26" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13" t="s">
         <v>129</v>
@@ -8744,10 +8962,17 @@
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
+      <c r="G27" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H27" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13" t="s">
         <v>130</v>
@@ -8757,10 +8982,17 @@
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="12"/>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
+      <c r="G28" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H28" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13" t="s">
         <v>105</v>
@@ -8770,10 +9002,17 @@
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="14"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+      <c r="G29" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H29" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13" t="s">
         <v>135</v>
@@ -8783,10 +9022,17 @@
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
+      <c r="G30" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H30" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13" t="s">
         <v>136</v>
@@ -8796,10 +9042,17 @@
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
+      <c r="G31" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H31" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13" t="s">
         <v>137</v>
@@ -8809,10 +9062,17 @@
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
+      <c r="G32" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H32" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13" t="s">
         <v>138</v>
@@ -8822,10 +9082,17 @@
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
+      <c r="G33" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H33" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13" t="s">
         <v>139</v>
@@ -8835,10 +9102,17 @@
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
+      <c r="G34" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H34" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13" t="s">
         <v>79</v>
@@ -8848,10 +9122,17 @@
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
-      <c r="G35" s="14"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
+      <c r="G35" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H35" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13" t="s">
         <v>140</v>
@@ -8861,10 +9142,17 @@
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
+      <c r="G36" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H36" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13" t="s">
         <v>141</v>
@@ -8874,9 +9162,17 @@
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H37" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="17"/>
       <c r="B38" s="15"/>
       <c r="C38" s="13" t="s">
         <v>78</v>
@@ -8886,9 +9182,17 @@
       </c>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G38" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H38" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="17"/>
       <c r="B39" s="15"/>
       <c r="C39" s="13" t="s">
         <v>142</v>
@@ -8898,9 +9202,17 @@
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
-      <c r="G39" s="14"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H39" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="17"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15" t="s">
         <v>106</v>
@@ -8908,9 +9220,17 @@
       <c r="D40" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G40" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H40" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15" t="s">
         <v>143</v>
@@ -8918,27 +9238,34 @@
       <c r="D41" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G41" s="14"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H41" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>